<commit_message>
gabriel - adicionando tabelas na pasta origin
</commit_message>
<xml_diff>
--- a/ingestao_de_dados/origens/catalogo_de_dados.xlsx
+++ b/ingestao_de_dados/origens/catalogo_de_dados.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28526"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gabriel\Desktop\distribuicao_profissao\distribuicao-de-profissoes\ingestao_de_dados\origens\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA4C1C76-2A77-4018-ACC1-AD59196B65C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
@@ -18,9 +24,140 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="42">
+  <si>
+    <t>Tabela</t>
+  </si>
+  <si>
+    <t>Coluna</t>
+  </si>
+  <si>
+    <t>Tipo do Dado</t>
+  </si>
+  <si>
+    <t>Descritivo do Campo</t>
+  </si>
+  <si>
+    <t>advogados_genero_brasil</t>
+  </si>
+  <si>
+    <t>Advogados(as)</t>
+  </si>
+  <si>
+    <t>SECCIONAL</t>
+  </si>
+  <si>
+    <t>Id único que identifica cada campo na tabela</t>
+  </si>
+  <si>
+    <t>Estagiários (as)</t>
+  </si>
+  <si>
+    <t>Suplementares</t>
+  </si>
+  <si>
+    <t>Consultor Estrangeiro</t>
+  </si>
+  <si>
+    <t>Feminino</t>
+  </si>
+  <si>
+    <t>Masculino</t>
+  </si>
+  <si>
+    <t>INT</t>
+  </si>
+  <si>
+    <t>Campo que registra a quantidade de suplementares no brasil (advogados que atuam em mais de um estado)</t>
+  </si>
+  <si>
+    <t>Campo que registra a quantidade de estrangeiros que atuam na área de advocacia no Brasil</t>
+  </si>
+  <si>
+    <t>Campo que regista a quantidade de advogados em atividade no Brasil</t>
+  </si>
+  <si>
+    <t>Campo que registra a quantidade de estágiarios de advocacia em atividade no Brasil</t>
+  </si>
+  <si>
+    <t>Campo que registra o número de mulheres de cada categoria</t>
+  </si>
+  <si>
+    <t>Campo que registra o número de homens de cada categoria</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Campo que registra o total de advogados em cada estado </t>
+  </si>
+  <si>
+    <t>contadores_genero_brasil</t>
+  </si>
+  <si>
+    <t>Estado</t>
+  </si>
+  <si>
+    <t>Contador</t>
+  </si>
+  <si>
+    <t>Técnico</t>
+  </si>
+  <si>
+    <t>Subtotal</t>
+  </si>
+  <si>
+    <t>VARCHAR (50)</t>
+  </si>
+  <si>
+    <t>Campo que registra a quantidade de técnicos de contabilidade de cada estado do país</t>
+  </si>
+  <si>
+    <t>Campo que registra a quantidade de contadores em cada estado do Brasil</t>
+  </si>
+  <si>
+    <t>Campo que registra por gênero separadamente a quantidade de contadores no Brasil</t>
+  </si>
+  <si>
+    <t>%</t>
+  </si>
+  <si>
+    <t>Campo que registra a % em relação a cada coluna</t>
+  </si>
+  <si>
+    <t>Campo que registra o total de contadores sem distinguir gêneros</t>
+  </si>
+  <si>
+    <t>CREA</t>
+  </si>
+  <si>
+    <t>Campo que registra o número de engenheiras no Brasil</t>
+  </si>
+  <si>
+    <t>Campo que registra o número de engenheiros no Brasil</t>
+  </si>
+  <si>
+    <t>Campo que registra o total de engenheiros (as) no país</t>
+  </si>
+  <si>
+    <t>engenheiros_genero_brasil</t>
+  </si>
+  <si>
+    <t>psicologos_genero_brasil</t>
+  </si>
+  <si>
+    <t>Campo que registra o número de psicólogos no Brasil</t>
+  </si>
+  <si>
+    <t>Campo que registra o número de psicólogas no Brasil</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -28,16 +165,41 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -45,12 +207,45 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thick">
+        <color rgb="FFF9F9F9"/>
+      </left>
+      <right/>
+      <top style="thick">
+        <color rgb="FFF9F9F9"/>
+      </top>
+      <bottom style="thick">
+        <color rgb="FFF9F9F9"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color rgb="FFF9F9F9"/>
+      </right>
+      <top style="thick">
+        <color rgb="FFF9F9F9"/>
+      </top>
+      <bottom style="thick">
+        <color rgb="FFF9F9F9"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -330,13 +525,329 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:D22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="2" width="18.140625" customWidth="1"/>
+    <col min="3" max="3" width="18.5703125" customWidth="1"/>
+    <col min="4" max="4" width="19.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" t="s">
+        <v>13</v>
+      </c>
+      <c r="D8" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>4</v>
+      </c>
+      <c r="B9" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9" t="s">
+        <v>13</v>
+      </c>
+      <c r="D9" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>22</v>
+      </c>
+      <c r="B10" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10" t="s">
+        <v>27</v>
+      </c>
+      <c r="D10" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>22</v>
+      </c>
+      <c r="B11" t="s">
+        <v>24</v>
+      </c>
+      <c r="C11" t="s">
+        <v>13</v>
+      </c>
+      <c r="D11" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" t="s">
+        <v>25</v>
+      </c>
+      <c r="C12" t="s">
+        <v>13</v>
+      </c>
+      <c r="D12" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>22</v>
+      </c>
+      <c r="B13" t="s">
+        <v>26</v>
+      </c>
+      <c r="C13" t="s">
+        <v>13</v>
+      </c>
+      <c r="D13" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>22</v>
+      </c>
+      <c r="B14" t="s">
+        <v>31</v>
+      </c>
+      <c r="C14" t="s">
+        <v>13</v>
+      </c>
+      <c r="D14" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>22</v>
+      </c>
+      <c r="B15" t="s">
+        <v>20</v>
+      </c>
+      <c r="C15" t="s">
+        <v>13</v>
+      </c>
+      <c r="D15" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>38</v>
+      </c>
+      <c r="B16" t="s">
+        <v>34</v>
+      </c>
+      <c r="C16" t="s">
+        <v>27</v>
+      </c>
+      <c r="D16" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>38</v>
+      </c>
+      <c r="B17" t="s">
+        <v>11</v>
+      </c>
+      <c r="C17" t="s">
+        <v>13</v>
+      </c>
+      <c r="D17" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>38</v>
+      </c>
+      <c r="B18" t="s">
+        <v>12</v>
+      </c>
+      <c r="C18" t="s">
+        <v>13</v>
+      </c>
+      <c r="D18" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>38</v>
+      </c>
+      <c r="B19" t="s">
+        <v>20</v>
+      </c>
+      <c r="C19" t="s">
+        <v>13</v>
+      </c>
+      <c r="D19" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>39</v>
+      </c>
+      <c r="B20" t="s">
+        <v>23</v>
+      </c>
+      <c r="C20" t="s">
+        <v>27</v>
+      </c>
+      <c r="D20" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>39</v>
+      </c>
+      <c r="B21" t="s">
+        <v>11</v>
+      </c>
+      <c r="C21" t="s">
+        <v>13</v>
+      </c>
+      <c r="D21" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>39</v>
+      </c>
+      <c r="B22" t="s">
+        <v>12</v>
+      </c>
+      <c r="C22" t="s">
+        <v>13</v>
+      </c>
+      <c r="D22" t="s">
+        <v>40</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
atualizando tabelas da pasta origin
</commit_message>
<xml_diff>
--- a/ingestao_de_dados/origens/catalogo_de_dados.xlsx
+++ b/ingestao_de_dados/origens/catalogo_de_dados.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gabriel\Desktop\distribuicao_profissao\distribuicao-de-profissoes\ingestao_de_dados\origens\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA4C1C76-2A77-4018-ACC1-AD59196B65C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B4B8314-3D8A-44DD-B506-4FA0CF13DE88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="26">
   <si>
     <t>Tabela</t>
   </si>
@@ -42,24 +42,6 @@
     <t>advogados_genero_brasil</t>
   </si>
   <si>
-    <t>Advogados(as)</t>
-  </si>
-  <si>
-    <t>SECCIONAL</t>
-  </si>
-  <si>
-    <t>Id único que identifica cada campo na tabela</t>
-  </si>
-  <si>
-    <t>Estagiários (as)</t>
-  </si>
-  <si>
-    <t>Suplementares</t>
-  </si>
-  <si>
-    <t>Consultor Estrangeiro</t>
-  </si>
-  <si>
     <t>Feminino</t>
   </si>
   <si>
@@ -69,95 +51,65 @@
     <t>INT</t>
   </si>
   <si>
-    <t>Campo que registra a quantidade de suplementares no brasil (advogados que atuam em mais de um estado)</t>
-  </si>
-  <si>
-    <t>Campo que registra a quantidade de estrangeiros que atuam na área de advocacia no Brasil</t>
-  </si>
-  <si>
-    <t>Campo que regista a quantidade de advogados em atividade no Brasil</t>
-  </si>
-  <si>
-    <t>Campo que registra a quantidade de estágiarios de advocacia em atividade no Brasil</t>
-  </si>
-  <si>
-    <t>Campo que registra o número de mulheres de cada categoria</t>
-  </si>
-  <si>
-    <t>Campo que registra o número de homens de cada categoria</t>
-  </si>
-  <si>
-    <t>Total</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Campo que registra o total de advogados em cada estado </t>
-  </si>
-  <si>
     <t>contadores_genero_brasil</t>
   </si>
   <si>
     <t>Estado</t>
   </si>
   <si>
-    <t>Contador</t>
-  </si>
-  <si>
-    <t>Técnico</t>
-  </si>
-  <si>
-    <t>Subtotal</t>
-  </si>
-  <si>
     <t>VARCHAR (50)</t>
   </si>
   <si>
-    <t>Campo que registra a quantidade de técnicos de contabilidade de cada estado do país</t>
-  </si>
-  <si>
-    <t>Campo que registra a quantidade de contadores em cada estado do Brasil</t>
-  </si>
-  <si>
-    <t>Campo que registra por gênero separadamente a quantidade de contadores no Brasil</t>
-  </si>
-  <si>
-    <t>%</t>
-  </si>
-  <si>
-    <t>Campo que registra a % em relação a cada coluna</t>
-  </si>
-  <si>
-    <t>Campo que registra o total de contadores sem distinguir gêneros</t>
-  </si>
-  <si>
     <t>CREA</t>
   </si>
   <si>
-    <t>Campo que registra o número de engenheiras no Brasil</t>
-  </si>
-  <si>
-    <t>Campo que registra o número de engenheiros no Brasil</t>
-  </si>
-  <si>
-    <t>Campo que registra o total de engenheiros (as) no país</t>
-  </si>
-  <si>
     <t>engenheiros_genero_brasil</t>
   </si>
   <si>
     <t>psicologos_genero_brasil</t>
   </si>
   <si>
-    <t>Campo que registra o número de psicólogos no Brasil</t>
-  </si>
-  <si>
-    <t>Campo que registra o número de psicólogas no Brasil</t>
+    <t>Campo que registra a quantidade de pessoas do gênero feminino atuando como advogadas em cada estado do Brasil</t>
+  </si>
+  <si>
+    <t>Campo que registra a quantidade de pessoas do gênero masculino atuando como advogados em cada estado do Brasil</t>
+  </si>
+  <si>
+    <t>Id único que identifica cada campo na tabela de advogados</t>
+  </si>
+  <si>
+    <t>Id único que identifica cada campo na tabela de contadores</t>
+  </si>
+  <si>
+    <t>Campo que registra a quantidade de contadoras do gênero feminino de cada estado do Brasil</t>
+  </si>
+  <si>
+    <t>Campo que registra a quantidade de contadores do gênero masculino de cada estado do Brasil</t>
+  </si>
+  <si>
+    <t>Id único que identifica cada campo na tabela de engenheiros</t>
+  </si>
+  <si>
+    <t>Campo que registra a quantia do gênero feminino atuando na área de engenheria de cada estado do Brasil</t>
+  </si>
+  <si>
+    <t>Campo que registra a quantia do gênero masculino atuando na área de engenheria de cada estado do Brasil</t>
+  </si>
+  <si>
+    <t>Id único que identifica cada campo na tabela de psicólogos</t>
+  </si>
+  <si>
+    <t>Campo que registra o número de psicólogos em cada estado do Brasil</t>
+  </si>
+  <si>
+    <t>Campo que registra o número de psicólogas em cada estado do Brasil</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -172,14 +124,8 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -192,14 +138,8 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFFF"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="3">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -207,45 +147,13 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thick">
-        <color rgb="FFF9F9F9"/>
-      </left>
-      <right/>
-      <top style="thick">
-        <color rgb="FFF9F9F9"/>
-      </top>
-      <bottom style="thick">
-        <color rgb="FFF9F9F9"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thick">
-        <color rgb="FFF9F9F9"/>
-      </right>
-      <top style="thick">
-        <color rgb="FFF9F9F9"/>
-      </top>
-      <bottom style="thick">
-        <color rgb="FFF9F9F9"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -526,10 +434,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D22"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -558,16 +466,16 @@
         <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C2" t="s">
-        <v>27</v>
+        <v>10</v>
       </c>
       <c r="D2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -575,63 +483,63 @@
         <v>5</v>
       </c>
       <c r="C3" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="D3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>8</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>4</v>
       </c>
       <c r="B5" t="s">
         <v>9</v>
       </c>
       <c r="C5" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="D5" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="B6" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C6" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="D6" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="B7" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="C7" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="D7" t="s">
         <v>18</v>
@@ -639,27 +547,27 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="B8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C8" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="D8" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="B9" t="s">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="C9" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="D9" t="s">
         <v>21</v>
@@ -667,184 +575,58 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" t="s">
+        <v>7</v>
+      </c>
+      <c r="D10" t="s">
         <v>22</v>
-      </c>
-      <c r="B10" t="s">
-        <v>23</v>
-      </c>
-      <c r="C10" t="s">
-        <v>27</v>
-      </c>
-      <c r="D10" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="B11" t="s">
-        <v>24</v>
+        <v>9</v>
       </c>
       <c r="C11" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="D11" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="B12" t="s">
+        <v>5</v>
+      </c>
+      <c r="C12" t="s">
+        <v>7</v>
+      </c>
+      <c r="D12" t="s">
         <v>25</v>
-      </c>
-      <c r="C12" t="s">
-        <v>13</v>
-      </c>
-      <c r="D12" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="B13" t="s">
-        <v>26</v>
+        <v>6</v>
       </c>
       <c r="C13" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="D13" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>22</v>
-      </c>
-      <c r="B14" t="s">
-        <v>31</v>
-      </c>
-      <c r="C14" t="s">
-        <v>13</v>
-      </c>
-      <c r="D14" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>22</v>
-      </c>
-      <c r="B15" t="s">
-        <v>20</v>
-      </c>
-      <c r="C15" t="s">
-        <v>13</v>
-      </c>
-      <c r="D15" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>38</v>
-      </c>
-      <c r="B16" t="s">
-        <v>34</v>
-      </c>
-      <c r="C16" t="s">
-        <v>27</v>
-      </c>
-      <c r="D16" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>38</v>
-      </c>
-      <c r="B17" t="s">
-        <v>11</v>
-      </c>
-      <c r="C17" t="s">
-        <v>13</v>
-      </c>
-      <c r="D17" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>38</v>
-      </c>
-      <c r="B18" t="s">
-        <v>12</v>
-      </c>
-      <c r="C18" t="s">
-        <v>13</v>
-      </c>
-      <c r="D18" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>38</v>
-      </c>
-      <c r="B19" t="s">
-        <v>20</v>
-      </c>
-      <c r="C19" t="s">
-        <v>13</v>
-      </c>
-      <c r="D19" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>39</v>
-      </c>
-      <c r="B20" t="s">
-        <v>23</v>
-      </c>
-      <c r="C20" t="s">
-        <v>27</v>
-      </c>
-      <c r="D20" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>39</v>
-      </c>
-      <c r="B21" t="s">
-        <v>11</v>
-      </c>
-      <c r="C21" t="s">
-        <v>13</v>
-      </c>
-      <c r="D21" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>39</v>
-      </c>
-      <c r="B22" t="s">
-        <v>12</v>
-      </c>
-      <c r="C22" t="s">
-        <v>13</v>
-      </c>
-      <c r="D22" t="s">
-        <v>40</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>